<commit_message>
initial load data working
</commit_message>
<xml_diff>
--- a/src/main/resources/static/meal-data-load.xlsx
+++ b/src/main/resources/static/meal-data-load.xlsx
@@ -19,7 +19,7 @@
     <t>Prep chicken with regular seasoning.  Chop lettuce.  Add sliced tomatoes, parmesan cheese, croutons and dressing.  Bake chicken on roast at 450 degrees for 16 minutes.  Slice chicken and add to salad.</t>
   </si>
   <si>
-    <t>Lettuce,tomato,parmesan cheese,caesar dressing, chicken breast, croutons</t>
+    <t>Lettuce-Refrigerator,tomato-Cabinet,parmesan cheese-Refrigerator,caesar dressing-Refrigerator, chicken breast-Refrigerator, croutons-Cabinet</t>
   </si>
   <si>
     <t>Salmon Greek Salad</t>
@@ -28,7 +28,7 @@
     <t>Slice salmon into filets.  Add salt and pepper for seasoning.  Roast salmon at 475 degrees for 15 minutes.  Chop lettuce and add cucumber, tomatoes, red onion, sweet green pepper, feta cheese, and chickpeas.  Add dressing.  Add salmon filet.</t>
   </si>
   <si>
-    <t>Salmon,lettuce,cucumber,tomato,feta cheese, red onion, sweet green pepper, chickpeas</t>
+    <t>Salmon-Refrigerator,lettuce-Refrigerator,cucumber-Refrigerator,tomato-Cabinet,feta cheese-Refrigerator, red onion-Refrigerator, sweet green pepper-Refrigerator, chickpeas-Cabinet</t>
   </si>
   <si>
     <t>Chipotle Chicken, Rice, Green Beans</t>
@@ -37,7 +37,7 @@
     <t>Prep chicken with chipotle seasoning.  Roast chicken at 450 degrees for 16 minutes.  Prepare rice in rice cooker.  Prepare green beans in steam oven.  Slice chicken and add over rice with side of green beans.</t>
   </si>
   <si>
-    <t>Chicken breast,basmati rice, green beans, chipotle seasoning</t>
+    <t>Chicken breast-Refrigerator,basmati rice-Cabinet, green beans-Freezer, chipotle seasoning-Cabinet</t>
   </si>
   <si>
     <t>Bison Salad</t>
@@ -46,7 +46,7 @@
     <t>Slice bison filets into strips.  Season with salt and pepper.  Fry on stove top on medium heat until cooked through.  Chop lettuce.  Add walnuts, strawberries and balsamic dressing.  Add strips over salad.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bison filet,salt,pepper,lettuce,walnuts,strawberries,balsamic c dressing </t>
+    <t xml:space="preserve">Bison filet-Refrigerator,salt-Cabinet,pepper-Cabinet,lettuce-Refrigerator,walnuts-Cabinet,strawberries-Refrgierator,balsamic dressing-Refrigerator </t>
   </si>
   <si>
     <t>Salmon, Quinoa, Asparagus</t>
@@ -55,7 +55,7 @@
     <t>Slice salmon into filets.  Season with salt and pepper.  Roast salmon at 475 degrees for 15 minutes.  Prep quinoa in rice cooker.  Place asparagus in oven with salmon approximately 7 minutes before timer completes.  Serve salmon over quinoa with asparagus on the side.</t>
   </si>
   <si>
-    <t>Salmon, salt, pepper, quinoa, asparagus</t>
+    <t>Salmon-Refrigerator, salt-Cabinet, pepper-Cabinet, quinoa-Cabinet, asparagus-Refrigerator</t>
   </si>
   <si>
     <t>Crab Cake, Baked Potato, Brussel Sprouts</t>
@@ -64,7 +64,7 @@
     <t>Prep baked potatoes with salt and pepper.  Roast bake potato for 45 minutes at 450 degrees.  Rotate potato half way through.  Roast crab cakes per package directions.  Prep Brussel sprouts with salt and pepper.  Place Brussel sprouts in oven with crab cakes approximately 7 minutes before timer completes.</t>
   </si>
   <si>
-    <t>Crab cakes,russett potato, butter, salt, pepper,brussel sprouts,</t>
+    <t>Crab cakes-Refrigerator,russett potato-Cabinet, butter-Refrigerator, salt-Cabinet, pepper-Cabinet,brussel sprouts-Refrigerator</t>
   </si>
   <si>
     <t>Maple Glazed Salmon, Quinoa, Peas</t>
@@ -73,7 +73,7 @@
     <t>Prepare marinade by mixing maple syrup, soy sauce, dijon mustard and minced garlic.  Soak salmon filets with marinade.  Roast salmon for 15 minutes on 475 degrees.  Prep quinoa in rice cooker.  Prep peas in steam oven.  Place salmon over quinoa with peas on the side.  Spoon extra marinade from cooking dish over filets.</t>
   </si>
   <si>
-    <t>Maple syrup, soy sauce, dijon mustard, garlic, salmon, quinoa, peas</t>
+    <t>Maple syrup-Cabinet, soy sauce-Refrigerator, dijon mustard-Refrigerator, garlic-Cabinet, Salmon-Refrigerator, quinoa-Cabinet, peas-Freezer</t>
   </si>
 </sst>
 </file>

</xml_diff>